<commit_message>
working out some bugs
</commit_message>
<xml_diff>
--- a/qdbm/data/profiles.xlsx
+++ b/qdbm/data/profiles.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DBLP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Profile: DBLP</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>Second Session</t>
-  </si>
-  <si>
-    <t>% Change CPU</t>
-  </si>
-  <si>
-    <t>% Change WALL</t>
   </si>
 </sst>
 </file>
@@ -80,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -146,7 +140,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -488,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -545,12 +539,8 @@
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
@@ -846,7 +836,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
idk i hate git
</commit_message>
<xml_diff>
--- a/qdbm/data/profiles.xlsx
+++ b/qdbm/data/profiles.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DBLP" sheetId="1" r:id="rId1"/>
+    <sheet name="Wordnet" sheetId="2" r:id="rId2"/>
+    <sheet name="Large Random Files" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Profile: DBLP</t>
   </si>
@@ -67,14 +69,84 @@
   </si>
   <si>
     <t>Second Session</t>
+  </si>
+  <si>
+    <t>Synsets</t>
+  </si>
+  <si>
+    <t>Find for each word, all other words in the same synset.</t>
+  </si>
+  <si>
+    <t>Old Way (load_dyn + indexed xsb query)</t>
+  </si>
+  <si>
+    <t>Loading Time:</t>
+  </si>
+  <si>
+    <t>Computing Time:</t>
+  </si>
+  <si>
+    <t>Total Time:</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>New Way: (create a b+ tree and query).</t>
+  </si>
+  <si>
+    <t>Building Time:</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Noticed some strange condition when running multiple b+ tree tests in a row with itermitted lockups in wall time.</t>
+  </si>
+  <si>
+    <t>Large Random Fact Files</t>
+  </si>
+  <si>
+    <t>Using the p(i, i) format, iterate over all facts.</t>
+  </si>
+  <si>
+    <t>Old Way</t>
+  </si>
+  <si>
+    <t>Use assert to load the facts, then p(_,_) to loop through them all.</t>
+  </si>
+  <si>
+    <t>Trial:</t>
+  </si>
+  <si>
+    <t>Loading time:</t>
+  </si>
+  <si>
+    <t>upper1000000_pattern(i,i)_xsb</t>
+  </si>
+  <si>
+    <t>File:</t>
+  </si>
+  <si>
+    <t>New Way</t>
+  </si>
+  <si>
+    <t>Load facts into a p/2 tree indexed on the first arg, then use btgetall to iterate over all entries.</t>
+  </si>
+  <si>
+    <t>Building time:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -117,12 +189,186 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -137,10 +383,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -482,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -842,4 +1108,564 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1.204</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1.252</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.153</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="G9" s="12">
+        <f>SUM(B9:F9)/5</f>
+        <v>1.2128000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.379</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.32</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="G10" s="14">
+        <f>SUM(B10:F10)/5</f>
+        <v>0.31879999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1">
+      <c r="A11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="15">
+        <f>SUM(B9:B10)</f>
+        <v>1.583</v>
+      </c>
+      <c r="C11" s="15">
+        <f>SUM(C9:C10)</f>
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="D11" s="15">
+        <f t="shared" ref="D11:F11" si="0">SUM(D9:D10)</f>
+        <v>1.4730000000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>1.4449999999999998</v>
+      </c>
+      <c r="F11" s="15">
+        <f t="shared" si="0"/>
+        <v>1.6119999999999999</v>
+      </c>
+      <c r="G11" s="16">
+        <f>SUM(B11:F11)/5</f>
+        <v>1.5315999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <f>SUM(B16:F16) / 5</f>
+        <v>0.1946</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1.198</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E17" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="F17" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="G17" s="9">
+        <f>SUM(B17:F17) / 5</f>
+        <v>0.24059999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="13">
+        <v>2.2610000000000001</v>
+      </c>
+      <c r="C18" s="13">
+        <v>2.1480000000000001</v>
+      </c>
+      <c r="D18" s="13">
+        <v>2.81</v>
+      </c>
+      <c r="E18" s="13">
+        <v>2.1720000000000002</v>
+      </c>
+      <c r="F18" s="13">
+        <v>2.1930000000000001</v>
+      </c>
+      <c r="G18" s="9">
+        <f>SUM(B18:F18)/5</f>
+        <v>2.3168000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="A19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="15">
+        <f>SUM(B16:B18)</f>
+        <v>4.4320000000000004</v>
+      </c>
+      <c r="C19" s="15">
+        <f>SUM(C16:C18)</f>
+        <v>2.149</v>
+      </c>
+      <c r="D19" s="15">
+        <f>SUM(D16:D18)</f>
+        <v>2.8109999999999999</v>
+      </c>
+      <c r="E19" s="15">
+        <f>SUM(E16:E18)</f>
+        <v>2.1739999999999999</v>
+      </c>
+      <c r="F19" s="15">
+        <f>SUM(F16:F18)</f>
+        <v>2.194</v>
+      </c>
+      <c r="G19" s="16">
+        <f>SUM(G16:G18)</f>
+        <v>2.7520000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="B11" formulaRange="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" thickBot="1">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="11">
+        <v>19.765999999999998</v>
+      </c>
+      <c r="C12" s="11">
+        <v>19.905999999999999</v>
+      </c>
+      <c r="D12" s="11">
+        <v>19.914000000000001</v>
+      </c>
+      <c r="E12" s="11">
+        <v>19.945</v>
+      </c>
+      <c r="F12" s="11">
+        <v>19.895</v>
+      </c>
+      <c r="G12" s="12">
+        <f>SUM(B12:F12)/5</f>
+        <v>19.885200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C13" s="13">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E13" s="13">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F13" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G13" s="14">
+        <f t="shared" ref="G13:G14" si="0">SUM(B13:F13)/5</f>
+        <v>5.3799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1">
+      <c r="A14" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15">
+        <f>SUM(B12:B13)</f>
+        <v>19.815999999999999</v>
+      </c>
+      <c r="C14" s="15">
+        <f t="shared" ref="C14:F14" si="1">SUM(C12:C13)</f>
+        <v>19.977</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="1"/>
+        <v>19.965</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="1"/>
+        <v>19.994</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="1"/>
+        <v>19.942999999999998</v>
+      </c>
+      <c r="G14" s="16">
+        <f t="shared" si="0"/>
+        <v>19.939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" thickBot="1">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>4</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="11">
+        <v>31.547000000000001</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12">
+        <f>SUM(B20:F20) / 5</f>
+        <v>6.3094000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0</v>
+      </c>
+      <c r="D21" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="F21" s="13">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14">
+        <f>SUM(B21:F21) / 5</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="13">
+        <v>5.4269999999999996</v>
+      </c>
+      <c r="C22" s="13">
+        <v>4.95</v>
+      </c>
+      <c r="D22" s="13">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E22" s="13">
+        <v>4.9509999999999996</v>
+      </c>
+      <c r="F22" s="13">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="G22" s="14">
+        <f>SUM(B22:F22) / 5</f>
+        <v>5.0547999999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" thickBot="1">
+      <c r="A23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="15">
+        <f>SUM(B20:B22)</f>
+        <v>37.012</v>
+      </c>
+      <c r="C23" s="15">
+        <f t="shared" ref="C23:G23" si="2">SUM(C20:C22)</f>
+        <v>4.95</v>
+      </c>
+      <c r="D23" s="15">
+        <f t="shared" si="2"/>
+        <v>4.9740000000000002</v>
+      </c>
+      <c r="E23" s="15">
+        <f t="shared" si="2"/>
+        <v>4.952</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="2"/>
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="G23" s="16">
+        <f>SUM(B23:F23) / 5</f>
+        <v>11.372200000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removed a change in xsb
</commit_message>
<xml_diff>
--- a/qdbm/data/profiles.xlsx
+++ b/qdbm/data/profiles.xlsx
@@ -1673,10 +1673,15 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
moving some things around
</commit_message>
<xml_diff>
--- a/qdbm/data/profiles.xlsx
+++ b/qdbm/data/profiles.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="141">
   <si>
     <t>Profile: DBLP</t>
   </si>
@@ -277,133 +277,175 @@
     <t>Total Entries:</t>
   </si>
   <si>
-    <t>d3xaa</t>
-  </si>
-  <si>
-    <t>d3xab</t>
-  </si>
-  <si>
-    <t>d3xac</t>
-  </si>
-  <si>
-    <t>d3xad</t>
-  </si>
-  <si>
-    <t>d3xae</t>
-  </si>
-  <si>
     <t>Segments:</t>
   </si>
   <si>
-    <t>d3xaf</t>
-  </si>
-  <si>
-    <t>d3xag</t>
-  </si>
-  <si>
-    <t>d3xah</t>
-  </si>
-  <si>
-    <t>d3xai</t>
-  </si>
-  <si>
-    <t>d3xaj</t>
-  </si>
-  <si>
-    <t>d3xak</t>
-  </si>
-  <si>
-    <t>d3xal</t>
-  </si>
-  <si>
-    <t>d3xam</t>
-  </si>
-  <si>
-    <t>d3xan</t>
-  </si>
-  <si>
-    <t>d3xao</t>
-  </si>
-  <si>
-    <t>d3xap</t>
-  </si>
-  <si>
-    <t>d3xaq</t>
-  </si>
-  <si>
-    <t>d3xar</t>
-  </si>
-  <si>
-    <t>d3xas</t>
-  </si>
-  <si>
-    <t>d3xat</t>
-  </si>
-  <si>
-    <t>d3xau</t>
-  </si>
-  <si>
-    <t>d3xav</t>
-  </si>
-  <si>
-    <t>d3xaw</t>
-  </si>
-  <si>
-    <t>d3xax</t>
-  </si>
-  <si>
-    <t>d3xay</t>
-  </si>
-  <si>
-    <t>d3xaz</t>
-  </si>
-  <si>
-    <t>d3xba</t>
-  </si>
-  <si>
-    <t>d3xbc</t>
-  </si>
-  <si>
-    <t>d3xbb</t>
-  </si>
-  <si>
-    <t>d3xbd</t>
-  </si>
-  <si>
-    <t>d3xbe</t>
-  </si>
-  <si>
-    <t>d3xbf</t>
-  </si>
-  <si>
     <t>d3-data-1</t>
   </si>
   <si>
-    <t>d3xbg</t>
-  </si>
-  <si>
-    <t>d3xbh</t>
-  </si>
-  <si>
-    <t>d3xbi</t>
-  </si>
-  <si>
-    <t>d3xbj</t>
-  </si>
-  <si>
-    <t>d3xbk</t>
-  </si>
-  <si>
-    <t>d3xbl</t>
-  </si>
-  <si>
-    <t>d3xbm</t>
-  </si>
-  <si>
-    <t>d3xbn</t>
-  </si>
-  <si>
-    <t>d3xbo</t>
+    <t>d4xpo (404)</t>
+  </si>
+  <si>
+    <t>d4xpn (403)</t>
+  </si>
+  <si>
+    <t>d4xpm (402)</t>
+  </si>
+  <si>
+    <t>Total Parse Time:</t>
+  </si>
+  <si>
+    <t>d4xpl (401)</t>
+  </si>
+  <si>
+    <t>d4xpk (400)</t>
+  </si>
+  <si>
+    <t>d4xpj (399)</t>
+  </si>
+  <si>
+    <t>d4xpi (398)</t>
+  </si>
+  <si>
+    <t>d4xph (397)</t>
+  </si>
+  <si>
+    <t>Total Build Time:</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Datahub</t>
+  </si>
+  <si>
+    <t>d3xbo (40)</t>
+  </si>
+  <si>
+    <t>d3xbn (39)</t>
+  </si>
+  <si>
+    <t>d3xbm (38)</t>
+  </si>
+  <si>
+    <t>d3xbl (37)</t>
+  </si>
+  <si>
+    <t>d3xbk (36)</t>
+  </si>
+  <si>
+    <t>d3xbj (35)</t>
+  </si>
+  <si>
+    <t>d3xbi (34)</t>
+  </si>
+  <si>
+    <t>d3xbh (33)</t>
+  </si>
+  <si>
+    <t>d3xbg (32)</t>
+  </si>
+  <si>
+    <t>d3xbf (31)</t>
+  </si>
+  <si>
+    <t>d3xbe (30)</t>
+  </si>
+  <si>
+    <t>d3xbd (29)</t>
+  </si>
+  <si>
+    <t>d3xbc (28)</t>
+  </si>
+  <si>
+    <t>d3xbb (27)</t>
+  </si>
+  <si>
+    <t>d3xba (26)</t>
+  </si>
+  <si>
+    <t>d3xaz (25)</t>
+  </si>
+  <si>
+    <t>d3xay (24)</t>
+  </si>
+  <si>
+    <t>d3xax (23)</t>
+  </si>
+  <si>
+    <t>d3xaw (22)</t>
+  </si>
+  <si>
+    <t>d3xav (21)</t>
+  </si>
+  <si>
+    <t>d3xau (20)</t>
+  </si>
+  <si>
+    <t>d3xat (19)</t>
+  </si>
+  <si>
+    <t>d3xas (18)</t>
+  </si>
+  <si>
+    <t>d3xar (17)</t>
+  </si>
+  <si>
+    <t>d3xaq (16)</t>
+  </si>
+  <si>
+    <t>d3xap (15)</t>
+  </si>
+  <si>
+    <t>d3xao (14)</t>
+  </si>
+  <si>
+    <t>d3xan (13)</t>
+  </si>
+  <si>
+    <t>d3xam (12)</t>
+  </si>
+  <si>
+    <t>d3xal (11)</t>
+  </si>
+  <si>
+    <t>d3xak (10)</t>
+  </si>
+  <si>
+    <t>d3xaj (9)</t>
+  </si>
+  <si>
+    <t>d3xai (8)</t>
+  </si>
+  <si>
+    <t>d3xah (7)</t>
+  </si>
+  <si>
+    <t>d3xag (6)</t>
+  </si>
+  <si>
+    <t>d3xaf (5)</t>
+  </si>
+  <si>
+    <t>d3xae (4)</t>
+  </si>
+  <si>
+    <t>d3xad (3)</t>
+  </si>
+  <si>
+    <t>d3xac (2)</t>
+  </si>
+  <si>
+    <t>d3xab (1)</t>
+  </si>
+  <si>
+    <t>d3xaa (0)</t>
   </si>
 </sst>
 </file>
@@ -487,12 +529,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="18">
@@ -757,7 +805,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -797,13 +845,10 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -811,6 +856,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -2329,10 +2390,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2711,1228 +2772,2409 @@
     </row>
     <row r="24" spans="1:13" ht="16" thickBot="1">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16" thickBot="1">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="38" t="s">
+      <c r="F25" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="45"/>
+      <c r="G25" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="39">
+      <c r="A26" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="47">
         <v>2.4870000000000001</v>
       </c>
-      <c r="C26" s="39">
+      <c r="C26" s="47">
         <v>6.91</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="47">
         <f>SUM(B26:C26)</f>
         <v>9.3970000000000002</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="48">
         <v>849970</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="48">
         <f>E26</f>
         <v>849970</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
+      <c r="G26" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="43"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="40">
-        <v>5.7628000000000004</v>
-      </c>
-      <c r="C27" s="40">
-        <v>22.146999999999998</v>
-      </c>
-      <c r="D27" s="40">
-        <f>C27+B27</f>
-        <v>27.909799999999997</v>
-      </c>
-      <c r="E27" s="42">
+      <c r="A27" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="51">
+        <v>1.88</v>
+      </c>
+      <c r="C27" s="51">
+        <v>182.18</v>
+      </c>
+      <c r="D27" s="51">
+        <f>SUM(B27:C27)</f>
+        <v>184.06</v>
+      </c>
+      <c r="E27" s="52">
+        <v>596583</v>
+      </c>
+      <c r="F27" s="52">
+        <f>F26+E27</f>
+        <v>1446553</v>
+      </c>
+      <c r="G27" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="43"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="51">
+        <v>6.702</v>
+      </c>
+      <c r="C28" s="51">
+        <v>2141.8389999999999</v>
+      </c>
+      <c r="D28" s="51">
+        <f>SUM(B28:C28)</f>
+        <v>2148.5410000000002</v>
+      </c>
+      <c r="E28" s="52">
         <v>2000000</v>
       </c>
-      <c r="F27" s="42">
-        <f>F26+E27</f>
-        <v>2849970</v>
-      </c>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="40">
-        <v>6.1909999999999998</v>
-      </c>
-      <c r="C28" s="40">
-        <v>183.126</v>
-      </c>
-      <c r="D28" s="40">
-        <v>52.5</v>
-      </c>
-      <c r="E28" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F28" s="42">
+      <c r="F28" s="52">
         <f t="shared" ref="F28:F52" si="1">F27+E28</f>
-        <v>4849970</v>
-      </c>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
+        <v>3446553</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="43"/>
       <c r="K28" t="s">
         <v>81</v>
       </c>
       <c r="M28">
         <f>AVERAGE(B26:B52)</f>
-        <v>4.2504</v>
+        <v>2.2445555555555554</v>
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="40">
-        <v>6.2590000000000003</v>
-      </c>
-      <c r="C29" s="40">
-        <v>71.835999999999999</v>
-      </c>
-      <c r="D29" s="40">
+      <c r="A29" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="51">
+        <v>6.7809999999999997</v>
+      </c>
+      <c r="C29" s="51">
+        <v>2930.7570000000001</v>
+      </c>
+      <c r="D29" s="51">
         <f>SUM(B29:C29)</f>
-        <v>78.094999999999999</v>
-      </c>
-      <c r="E29" s="42">
+        <v>2937.538</v>
+      </c>
+      <c r="E29" s="52">
         <v>2000000</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="52">
         <f t="shared" si="1"/>
-        <v>6849970</v>
-      </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
+        <v>5446553</v>
+      </c>
+      <c r="G29" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="43"/>
       <c r="K29" t="s">
         <v>82</v>
       </c>
       <c r="M29">
         <f>AVERAGE(C26:C52)</f>
-        <v>414.19103703703706</v>
+        <v>455.62118518518531</v>
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="40">
-        <v>6.0919999999999996</v>
-      </c>
-      <c r="C30" s="40">
-        <v>74.933999999999997</v>
-      </c>
-      <c r="D30" s="40">
+      <c r="A30" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="51">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="C30" s="51">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D30" s="51">
         <f>SUM(B30:C30)</f>
-        <v>81.025999999999996</v>
-      </c>
-      <c r="E30" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F30" s="42">
+        <v>0.628</v>
+      </c>
+      <c r="E30" s="53">
+        <v>96</v>
+      </c>
+      <c r="F30" s="52">
         <f t="shared" si="1"/>
-        <v>8849970</v>
-      </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
+        <v>5446649</v>
+      </c>
+      <c r="G30" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="45"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="40">
-        <v>6.26</v>
-      </c>
-      <c r="C31" s="40">
-        <v>276.38099999999997</v>
-      </c>
-      <c r="D31" s="40">
-        <f t="shared" ref="D31:D52" si="2">SUM(B31:C31)</f>
-        <v>282.64099999999996</v>
-      </c>
-      <c r="E31" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F31" s="42">
+      <c r="A31" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="51">
+        <v>1.2450000000000001</v>
+      </c>
+      <c r="C31" s="51">
+        <v>395.67700000000002</v>
+      </c>
+      <c r="D31" s="51">
+        <f>SUM(B31:C31)</f>
+        <v>396.92200000000003</v>
+      </c>
+      <c r="E31" s="53">
+        <v>266053</v>
+      </c>
+      <c r="F31" s="52">
         <f t="shared" si="1"/>
-        <v>10849970</v>
-      </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="48"/>
+        <v>5712702</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="45"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="40">
-        <v>6.181</v>
-      </c>
-      <c r="C32" s="40">
-        <v>103.024</v>
-      </c>
-      <c r="D32" s="40">
-        <f t="shared" si="2"/>
-        <v>109.205</v>
-      </c>
-      <c r="E32" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F32" s="42">
+      <c r="A32" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="51">
+        <v>1.0840000000000001</v>
+      </c>
+      <c r="C32" s="51">
+        <v>76.88</v>
+      </c>
+      <c r="D32" s="51">
+        <f>SUM(B32:C32)</f>
+        <v>77.963999999999999</v>
+      </c>
+      <c r="E32" s="53">
+        <v>211024</v>
+      </c>
+      <c r="F32" s="52">
         <f t="shared" si="1"/>
-        <v>12849970</v>
-      </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="48"/>
+        <v>5923726</v>
+      </c>
+      <c r="G32" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="45"/>
       <c r="I32" s="2"/>
       <c r="K32" t="s">
         <v>83</v>
       </c>
       <c r="M32" s="33">
         <f>SUM(E26:E52)</f>
-        <v>34103300</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="40">
-        <v>6.5540000000000003</v>
-      </c>
-      <c r="C33" s="40">
-        <v>588.47400000000005</v>
-      </c>
-      <c r="D33" s="40">
-        <f t="shared" si="2"/>
-        <v>595.02800000000002</v>
-      </c>
-      <c r="E33" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F33" s="42">
+        <v>17048533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="51">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="C33" s="51">
+        <v>131.84700000000001</v>
+      </c>
+      <c r="D33" s="51">
+        <f>SUM(B33:C33)</f>
+        <v>132.72800000000001</v>
+      </c>
+      <c r="E33" s="53">
+        <v>272858</v>
+      </c>
+      <c r="F33" s="52">
         <f t="shared" si="1"/>
-        <v>14849970</v>
-      </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="48"/>
+        <v>6196584</v>
+      </c>
+      <c r="G33" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33" s="45"/>
       <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="40">
-        <v>6.6390000000000002</v>
-      </c>
-      <c r="C34" s="40">
-        <v>1076.6959999999999</v>
-      </c>
-      <c r="D34" s="40">
-        <f t="shared" si="2"/>
-        <v>1083.3349999999998</v>
-      </c>
-      <c r="E34" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F34" s="42">
+      <c r="K33" t="s">
+        <v>89</v>
+      </c>
+      <c r="M33" s="2">
+        <f>SUM(B26:B147) / 60</f>
+        <v>2.9108299999999994</v>
+      </c>
+      <c r="N33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="51">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C34" s="51">
+        <v>105.878</v>
+      </c>
+      <c r="D34" s="51">
+        <f>SUM(B34:C34)</f>
+        <v>106.575</v>
+      </c>
+      <c r="E34" s="53">
+        <v>203451</v>
+      </c>
+      <c r="F34" s="52">
         <f t="shared" si="1"/>
-        <v>16849970</v>
-      </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="48"/>
+        <v>6400035</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="45"/>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="40">
-        <v>6.8319999999999999</v>
-      </c>
-      <c r="C35" s="40">
-        <v>920.74599999999998</v>
-      </c>
-      <c r="D35" s="40">
-        <f t="shared" si="2"/>
-        <v>927.57799999999997</v>
-      </c>
-      <c r="E35" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F35" s="42">
+      <c r="K34" t="s">
+        <v>95</v>
+      </c>
+      <c r="M34" s="2">
+        <f>SUM(C26:C148) / (60 * 60)</f>
+        <v>5.9558455555555563</v>
+      </c>
+      <c r="N34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="51">
+        <v>4.45</v>
+      </c>
+      <c r="C35" s="51">
+        <v>920.50599999999997</v>
+      </c>
+      <c r="D35" s="51">
+        <f>SUM(B35:C35)</f>
+        <v>924.95600000000002</v>
+      </c>
+      <c r="E35" s="53">
+        <v>1392940</v>
+      </c>
+      <c r="F35" s="52">
         <f t="shared" si="1"/>
-        <v>18849970</v>
-      </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
+        <v>7792975</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="45"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="40">
-        <v>2.694</v>
-      </c>
-      <c r="C36" s="40">
-        <v>131.821</v>
-      </c>
-      <c r="D36" s="40">
-        <f t="shared" si="2"/>
-        <v>134.51499999999999</v>
-      </c>
-      <c r="E36" s="43">
-        <v>521186</v>
-      </c>
-      <c r="F36" s="42">
+    <row r="36" spans="1:14">
+      <c r="A36" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="51">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="C36" s="51">
+        <v>235.67099999999999</v>
+      </c>
+      <c r="D36" s="51">
+        <f>SUM(B36:C36)</f>
+        <v>237.38399999999999</v>
+      </c>
+      <c r="E36" s="53">
+        <v>529132</v>
+      </c>
+      <c r="F36" s="52">
         <f t="shared" si="1"/>
-        <v>19371156</v>
-      </c>
-      <c r="G36" s="47"/>
-      <c r="H36" s="48"/>
+        <v>8322107</v>
+      </c>
+      <c r="G36" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="45"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="40">
-        <v>6.8529999999999998</v>
-      </c>
-      <c r="C37" s="40">
-        <v>672.69200000000001</v>
-      </c>
-      <c r="D37" s="40">
-        <f t="shared" si="2"/>
-        <v>679.54499999999996</v>
-      </c>
-      <c r="E37" s="42">
-        <v>2000000</v>
-      </c>
-      <c r="F37" s="42">
+    <row r="37" spans="1:14">
+      <c r="A37" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="51">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="C37" s="51">
+        <v>146.08799999999999</v>
+      </c>
+      <c r="D37" s="51">
+        <f>SUM(B37:C37)</f>
+        <v>146.995</v>
+      </c>
+      <c r="E37" s="53">
+        <v>292817</v>
+      </c>
+      <c r="F37" s="52">
         <f t="shared" si="1"/>
-        <v>21371156</v>
-      </c>
-      <c r="G37" s="47"/>
-      <c r="H37" s="48"/>
+        <v>8614924</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H37" s="45"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="40">
-        <v>5.4660000000000002</v>
-      </c>
-      <c r="C38" s="40">
-        <v>488.24200000000002</v>
-      </c>
-      <c r="D38" s="40">
-        <f t="shared" si="2"/>
-        <v>493.70800000000003</v>
-      </c>
-      <c r="E38" s="43">
-        <v>1615295</v>
-      </c>
-      <c r="F38" s="42">
+    <row r="38" spans="1:14">
+      <c r="A38" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="51">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="C38" s="51">
+        <v>24.056999999999999</v>
+      </c>
+      <c r="D38" s="51">
+        <f>SUM(B38:C38)</f>
+        <v>24.475999999999999</v>
+      </c>
+      <c r="E38" s="53">
+        <v>126346</v>
+      </c>
+      <c r="F38" s="52">
         <f t="shared" si="1"/>
-        <v>22986451</v>
-      </c>
-      <c r="G38" s="47"/>
-      <c r="H38" s="48"/>
+        <v>8741270</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" s="45"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="40">
-        <v>2.085</v>
-      </c>
-      <c r="C39" s="40">
-        <v>607.57500000000005</v>
-      </c>
-      <c r="D39" s="40">
-        <f t="shared" si="2"/>
-        <v>609.66000000000008</v>
-      </c>
-      <c r="E39" s="43">
-        <v>520875</v>
-      </c>
-      <c r="F39" s="42">
+    <row r="39" spans="1:14">
+      <c r="A39" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="51">
+        <v>7.8E-2</v>
+      </c>
+      <c r="C39" s="51">
+        <v>3.6080000000000001</v>
+      </c>
+      <c r="D39" s="51">
+        <f>SUM(B39:C39)</f>
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="E39" s="53">
+        <v>15407</v>
+      </c>
+      <c r="F39" s="52">
         <f t="shared" si="1"/>
-        <v>23507326</v>
-      </c>
-      <c r="G39" s="47"/>
-      <c r="H39" s="48"/>
+        <v>8756677</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H39" s="45"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="40">
-        <v>3.1880000000000002</v>
-      </c>
-      <c r="C40" s="40">
-        <v>445.346</v>
-      </c>
-      <c r="D40" s="40">
-        <f t="shared" si="2"/>
-        <v>448.53399999999999</v>
-      </c>
-      <c r="E40" s="43">
-        <v>886999</v>
-      </c>
-      <c r="F40" s="42">
+    <row r="40" spans="1:14">
+      <c r="A40" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="51">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C40" s="51">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="D40" s="51">
+        <f>SUM(B40:C40)</f>
+        <v>9.1910000000000007</v>
+      </c>
+      <c r="E40" s="53">
+        <v>44036</v>
+      </c>
+      <c r="F40" s="52">
         <f t="shared" si="1"/>
-        <v>24394325</v>
-      </c>
-      <c r="G40" s="47"/>
-      <c r="H40" s="48"/>
+        <v>8800713</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H40" s="45"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="34" t="s">
+    <row r="41" spans="1:14">
+      <c r="A41" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="51">
+        <v>0.126</v>
+      </c>
+      <c r="C41" s="51">
+        <v>27.026</v>
+      </c>
+      <c r="D41" s="51">
+        <f>SUM(B41:C41)</f>
+        <v>27.152000000000001</v>
+      </c>
+      <c r="E41" s="53">
+        <v>30815</v>
+      </c>
+      <c r="F41" s="52">
+        <f t="shared" si="1"/>
+        <v>8831528</v>
+      </c>
+      <c r="G41" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="40">
-        <v>4.7190000000000003</v>
-      </c>
-      <c r="C41" s="40">
-        <v>549.524</v>
-      </c>
-      <c r="D41" s="40">
-        <f t="shared" si="2"/>
-        <v>554.24300000000005</v>
-      </c>
-      <c r="E41" s="43">
-        <v>1491970</v>
-      </c>
-      <c r="F41" s="42">
+      <c r="H41" s="45"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="51">
+        <v>1.1639999999999999</v>
+      </c>
+      <c r="C42" s="51">
+        <v>109.416</v>
+      </c>
+      <c r="D42" s="51">
+        <f>SUM(B42:C42)</f>
+        <v>110.58</v>
+      </c>
+      <c r="E42" s="53">
+        <v>236414</v>
+      </c>
+      <c r="F42" s="52">
         <f t="shared" si="1"/>
-        <v>25886295</v>
-      </c>
-      <c r="G41" s="47"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="40">
-        <v>4.7649999999999997</v>
-      </c>
-      <c r="C42" s="40">
-        <v>610.79499999999996</v>
-      </c>
-      <c r="D42" s="40">
-        <f t="shared" si="2"/>
-        <v>615.55999999999995</v>
-      </c>
-      <c r="E42" s="43">
-        <v>1397938</v>
-      </c>
-      <c r="F42" s="42">
+        <v>9067942</v>
+      </c>
+      <c r="G42" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="45"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="51">
+        <v>3.6779999999999999</v>
+      </c>
+      <c r="C43" s="51">
+        <v>548.72</v>
+      </c>
+      <c r="D43" s="51">
+        <f>SUM(B43:C43)</f>
+        <v>552.39800000000002</v>
+      </c>
+      <c r="E43" s="53">
+        <v>1062279</v>
+      </c>
+      <c r="F43" s="52">
         <f t="shared" si="1"/>
-        <v>27284233</v>
-      </c>
-      <c r="G42" s="47"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="40">
-        <v>4.3929999999999998</v>
-      </c>
-      <c r="C43" s="40">
-        <v>666.87800000000004</v>
-      </c>
-      <c r="D43" s="40">
-        <f t="shared" si="2"/>
-        <v>671.27100000000007</v>
-      </c>
-      <c r="E43" s="43">
-        <v>1271812</v>
-      </c>
-      <c r="F43" s="42">
+        <v>10130221</v>
+      </c>
+      <c r="G43" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H43" s="45"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="51">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="C44" s="51">
+        <v>160.173</v>
+      </c>
+      <c r="D44" s="51">
+        <f>SUM(B44:C44)</f>
+        <v>161.745</v>
+      </c>
+      <c r="E44" s="53">
+        <v>366779</v>
+      </c>
+      <c r="F44" s="52">
         <f t="shared" si="1"/>
-        <v>28556045</v>
-      </c>
-      <c r="G43" s="47"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="40">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="C44" s="40">
-        <v>17.829999999999998</v>
-      </c>
-      <c r="D44" s="40">
-        <f t="shared" si="2"/>
-        <v>18.376999999999999</v>
-      </c>
-      <c r="E44" s="43">
-        <v>33935</v>
-      </c>
-      <c r="F44" s="42">
-        <f t="shared" si="1"/>
-        <v>28589980</v>
-      </c>
-      <c r="G44" s="47"/>
-      <c r="H44" s="48"/>
+        <v>10497000</v>
+      </c>
+      <c r="G44" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" s="45"/>
       <c r="I44" s="2"/>
       <c r="K44" s="33"/>
     </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="40">
+    <row r="45" spans="1:14">
+      <c r="A45" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="51">
+        <v>2.2650000000000001</v>
+      </c>
+      <c r="C45" s="51">
+        <v>423.18599999999998</v>
+      </c>
+      <c r="D45" s="51">
+        <f>SUM(B45:C45)</f>
+        <v>425.45099999999996</v>
+      </c>
+      <c r="E45" s="53">
+        <v>597068</v>
+      </c>
+      <c r="F45" s="52">
+        <f t="shared" si="1"/>
+        <v>11094068</v>
+      </c>
+      <c r="G45" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H45" s="45"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="51">
+        <v>2.1909999999999998</v>
+      </c>
+      <c r="C46" s="51">
+        <v>597.00400000000002</v>
+      </c>
+      <c r="D46" s="51">
+        <f>SUM(B46:C46)</f>
+        <v>599.19500000000005</v>
+      </c>
+      <c r="E46" s="53">
+        <v>401348</v>
+      </c>
+      <c r="F46" s="52">
+        <f t="shared" si="1"/>
+        <v>11495416</v>
+      </c>
+      <c r="G46" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H46" s="45"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="51">
+        <v>6.7679999999999998</v>
+      </c>
+      <c r="C47" s="51">
+        <v>1364.4</v>
+      </c>
+      <c r="D47" s="51">
+        <f>SUM(B47:C47)</f>
+        <v>1371.1680000000001</v>
+      </c>
+      <c r="E47" s="52">
+        <v>2000000</v>
+      </c>
+      <c r="F47" s="52">
+        <f t="shared" si="1"/>
+        <v>13495416</v>
+      </c>
+      <c r="G47" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" s="45"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="51">
+        <v>2.056</v>
+      </c>
+      <c r="C48" s="51">
+        <v>379.43</v>
+      </c>
+      <c r="D48" s="51">
+        <f>SUM(B48:C48)</f>
+        <v>381.48599999999999</v>
+      </c>
+      <c r="E48" s="53">
+        <v>654911</v>
+      </c>
+      <c r="F48" s="52">
+        <f t="shared" si="1"/>
+        <v>14150327</v>
+      </c>
+      <c r="G48" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H48" s="45"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="51">
         <v>1.099</v>
       </c>
-      <c r="C45" s="40">
+      <c r="C49" s="51">
         <v>85.852000000000004</v>
       </c>
-      <c r="D45" s="40">
-        <f t="shared" si="2"/>
+      <c r="D49" s="51">
+        <f>SUM(B49:C49)</f>
         <v>86.951000000000008</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E49" s="53">
         <v>194521</v>
       </c>
-      <c r="F45" s="42">
+      <c r="F49" s="52">
         <f t="shared" si="1"/>
-        <v>28784501</v>
-      </c>
-      <c r="G45" s="47"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="B46" s="40">
-        <v>2.056</v>
-      </c>
-      <c r="C46" s="40">
-        <v>379.43</v>
-      </c>
-      <c r="D46" s="40">
-        <f t="shared" si="2"/>
-        <v>381.48599999999999</v>
-      </c>
-      <c r="E46" s="43">
-        <v>654911</v>
-      </c>
-      <c r="F46" s="42">
+        <v>14344848</v>
+      </c>
+      <c r="G49" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="45"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="51">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="C50" s="51">
+        <v>17.829999999999998</v>
+      </c>
+      <c r="D50" s="51">
+        <f>SUM(B50:C50)</f>
+        <v>18.376999999999999</v>
+      </c>
+      <c r="E50" s="53">
+        <v>33935</v>
+      </c>
+      <c r="F50" s="52">
         <f t="shared" si="1"/>
-        <v>29439412</v>
-      </c>
-      <c r="G46" s="47"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="40">
-        <v>6.7679999999999998</v>
-      </c>
-      <c r="C47" s="40">
-        <v>1364.4</v>
-      </c>
-      <c r="D47" s="40">
-        <f t="shared" si="2"/>
-        <v>1371.1680000000001</v>
-      </c>
-      <c r="E47" s="42">
+        <v>14378783</v>
+      </c>
+      <c r="G50" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" s="45"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" s="51">
+        <v>4.3929999999999998</v>
+      </c>
+      <c r="C51" s="51">
+        <v>666.87800000000004</v>
+      </c>
+      <c r="D51" s="51">
+        <f>SUM(B51:C51)</f>
+        <v>671.27100000000007</v>
+      </c>
+      <c r="E51" s="53">
+        <v>1271812</v>
+      </c>
+      <c r="F51" s="52">
+        <f t="shared" si="1"/>
+        <v>15650595</v>
+      </c>
+      <c r="G51" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H51" s="45"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="51">
+        <v>4.7649999999999997</v>
+      </c>
+      <c r="C52" s="51">
+        <v>610.79499999999996</v>
+      </c>
+      <c r="D52" s="51">
+        <f>SUM(B52:C52)</f>
+        <v>615.55999999999995</v>
+      </c>
+      <c r="E52" s="53">
+        <v>1397938</v>
+      </c>
+      <c r="F52" s="52">
+        <f t="shared" si="1"/>
+        <v>17048533</v>
+      </c>
+      <c r="G52" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52" s="45"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" s="51">
+        <v>4.7190000000000003</v>
+      </c>
+      <c r="C53" s="51">
+        <v>549.524</v>
+      </c>
+      <c r="D53" s="51">
+        <f>SUM(B53:C53)</f>
+        <v>554.24300000000005</v>
+      </c>
+      <c r="E53" s="53">
+        <v>1491970</v>
+      </c>
+      <c r="F53" s="52">
+        <f t="shared" ref="F53" si="2">F52+E53</f>
+        <v>18540503</v>
+      </c>
+      <c r="G53" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H53" s="45"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="51">
+        <v>3.1880000000000002</v>
+      </c>
+      <c r="C54" s="51">
+        <v>445.346</v>
+      </c>
+      <c r="D54" s="51">
+        <f>SUM(B54:C54)</f>
+        <v>448.53399999999999</v>
+      </c>
+      <c r="E54" s="53">
+        <v>886999</v>
+      </c>
+      <c r="F54" s="52">
+        <f t="shared" ref="F54:F76" si="3">F53+E54</f>
+        <v>19427502</v>
+      </c>
+      <c r="G54" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H54" s="45"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="51">
+        <v>2.085</v>
+      </c>
+      <c r="C55" s="51">
+        <v>607.57500000000005</v>
+      </c>
+      <c r="D55" s="51">
+        <f>SUM(B55:C55)</f>
+        <v>609.66000000000008</v>
+      </c>
+      <c r="E55" s="53">
+        <v>520875</v>
+      </c>
+      <c r="F55" s="52">
+        <f t="shared" si="3"/>
+        <v>19948377</v>
+      </c>
+      <c r="G55" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H55" s="45"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="55">
+        <v>5.4660000000000002</v>
+      </c>
+      <c r="C56" s="55">
+        <v>488.24200000000002</v>
+      </c>
+      <c r="D56" s="55">
+        <f>SUM(B56:C56)</f>
+        <v>493.70800000000003</v>
+      </c>
+      <c r="E56" s="56">
+        <v>1615295</v>
+      </c>
+      <c r="F56" s="57">
+        <f t="shared" si="3"/>
+        <v>21563672</v>
+      </c>
+      <c r="G56" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="H56" s="45"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="60">
+        <v>6.8529999999999998</v>
+      </c>
+      <c r="C57" s="60">
+        <v>672.69200000000001</v>
+      </c>
+      <c r="D57" s="60">
+        <f>SUM(B57:C57)</f>
+        <v>679.54499999999996</v>
+      </c>
+      <c r="E57" s="61">
         <v>2000000</v>
       </c>
-      <c r="F47" s="42">
-        <f t="shared" si="1"/>
-        <v>31439412</v>
-      </c>
-      <c r="G47" s="47"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="40">
-        <v>2.1909999999999998</v>
-      </c>
-      <c r="C48" s="40">
-        <v>597.00400000000002</v>
-      </c>
-      <c r="D48" s="40">
-        <f t="shared" si="2"/>
-        <v>599.19500000000005</v>
-      </c>
-      <c r="E48" s="43">
-        <v>401348</v>
-      </c>
-      <c r="F48" s="42">
-        <f t="shared" si="1"/>
-        <v>31840760</v>
-      </c>
-      <c r="G48" s="47"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="2"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="40">
-        <v>2.2650000000000001</v>
-      </c>
-      <c r="C49" s="40">
-        <v>423.18599999999998</v>
-      </c>
-      <c r="D49" s="40">
-        <f t="shared" si="2"/>
-        <v>425.45099999999996</v>
-      </c>
-      <c r="E49" s="43">
-        <v>597068</v>
-      </c>
-      <c r="F49" s="42">
-        <f t="shared" si="1"/>
-        <v>32437828</v>
-      </c>
-      <c r="G49" s="47"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="40">
-        <v>1.5720000000000001</v>
-      </c>
-      <c r="C50" s="40">
-        <v>160.173</v>
-      </c>
-      <c r="D50" s="40">
-        <f t="shared" si="2"/>
-        <v>161.745</v>
-      </c>
-      <c r="E50" s="43">
-        <v>366779</v>
-      </c>
-      <c r="F50" s="42">
-        <f t="shared" si="1"/>
-        <v>32804607</v>
-      </c>
-      <c r="G50" s="47"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51" s="40">
-        <v>3.6779999999999999</v>
-      </c>
-      <c r="C51" s="40">
-        <v>548.72</v>
-      </c>
-      <c r="D51" s="40">
-        <f t="shared" si="2"/>
-        <v>552.39800000000002</v>
-      </c>
-      <c r="E51" s="43">
-        <v>1062279</v>
-      </c>
-      <c r="F51" s="42">
-        <f t="shared" si="1"/>
-        <v>33866886</v>
-      </c>
-      <c r="G51" s="47"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" s="40">
-        <v>1.1639999999999999</v>
-      </c>
-      <c r="C52" s="40">
-        <v>109.416</v>
-      </c>
-      <c r="D52" s="40">
-        <f t="shared" si="2"/>
-        <v>110.58</v>
-      </c>
-      <c r="E52" s="43">
-        <v>236414</v>
-      </c>
-      <c r="F52" s="42">
-        <f t="shared" si="1"/>
-        <v>34103300</v>
-      </c>
-      <c r="G52" s="47"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="40">
-        <v>0.126</v>
-      </c>
-      <c r="C53" s="40">
-        <v>27.026</v>
-      </c>
-      <c r="D53" s="40">
-        <f t="shared" ref="D53" si="3">SUM(B53:C53)</f>
-        <v>27.152000000000001</v>
-      </c>
-      <c r="E53" s="43">
-        <v>30815</v>
-      </c>
-      <c r="F53" s="42">
-        <f t="shared" ref="F53" si="4">F52+E53</f>
-        <v>34134115</v>
-      </c>
-      <c r="G53" s="47"/>
-      <c r="H53" s="48"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="40">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="C54" s="40">
-        <v>9.0150000000000006</v>
-      </c>
-      <c r="D54" s="40">
-        <f t="shared" ref="D54:D76" si="5">SUM(B54:C54)</f>
-        <v>9.1910000000000007</v>
-      </c>
-      <c r="E54" s="43">
-        <v>44036</v>
-      </c>
-      <c r="F54" s="42">
-        <f t="shared" ref="F54:F76" si="6">F53+E54</f>
-        <v>34178151</v>
-      </c>
-      <c r="G54" s="47"/>
-      <c r="H54" s="48"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" s="40">
-        <v>7.8E-2</v>
-      </c>
-      <c r="C55" s="40">
-        <v>3.6080000000000001</v>
-      </c>
-      <c r="D55" s="40">
-        <f t="shared" si="5"/>
-        <v>3.6859999999999999</v>
-      </c>
-      <c r="E55" s="43">
-        <v>15407</v>
-      </c>
-      <c r="F55" s="42">
-        <f t="shared" si="6"/>
-        <v>34193558</v>
-      </c>
-      <c r="G55" s="47"/>
-      <c r="H55" s="48"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B56" s="40">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="C56" s="40">
-        <v>24.056999999999999</v>
-      </c>
-      <c r="D56" s="40">
-        <f t="shared" si="5"/>
-        <v>24.475999999999999</v>
-      </c>
-      <c r="E56" s="43">
-        <v>126346</v>
-      </c>
-      <c r="F56" s="42">
-        <f t="shared" si="6"/>
-        <v>34319904</v>
-      </c>
-      <c r="G56" s="47"/>
-      <c r="H56" s="48"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="40">
-        <v>0.90700000000000003</v>
-      </c>
-      <c r="C57" s="40">
-        <v>146.08799999999999</v>
-      </c>
-      <c r="D57" s="40">
-        <f t="shared" si="5"/>
-        <v>146.995</v>
-      </c>
-      <c r="E57" s="43">
-        <v>292817</v>
-      </c>
-      <c r="F57" s="42">
-        <f t="shared" si="6"/>
-        <v>34612721</v>
-      </c>
-      <c r="G57" s="47"/>
-      <c r="H57" s="48"/>
+      <c r="F57" s="61">
+        <f t="shared" si="3"/>
+        <v>23563672</v>
+      </c>
+      <c r="G57" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H57" s="45"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="40">
-        <v>1.7130000000000001</v>
-      </c>
-      <c r="C58" s="40">
-        <v>235.67099999999999</v>
-      </c>
-      <c r="D58" s="40">
-        <f t="shared" si="5"/>
-        <v>237.38399999999999</v>
-      </c>
-      <c r="E58" s="43">
-        <v>529132</v>
-      </c>
-      <c r="F58" s="42">
-        <f t="shared" si="6"/>
-        <v>35141853</v>
-      </c>
-      <c r="G58" s="47"/>
-      <c r="H58" s="48"/>
+        <v>131</v>
+      </c>
+      <c r="B58" s="38">
+        <v>2.694</v>
+      </c>
+      <c r="C58" s="38">
+        <v>131.821</v>
+      </c>
+      <c r="D58" s="38">
+        <f>SUM(B58:C58)</f>
+        <v>134.51499999999999</v>
+      </c>
+      <c r="E58" s="40">
+        <v>521186</v>
+      </c>
+      <c r="F58" s="39">
+        <f t="shared" si="3"/>
+        <v>24084858</v>
+      </c>
+      <c r="G58" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H58" s="45"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="40">
-        <v>4.45</v>
-      </c>
-      <c r="C59" s="40">
-        <v>920.50599999999997</v>
-      </c>
-      <c r="D59" s="40">
-        <f t="shared" si="5"/>
-        <v>924.95600000000002</v>
-      </c>
-      <c r="E59" s="43">
-        <v>1392940</v>
-      </c>
-      <c r="F59" s="42">
-        <f t="shared" si="6"/>
-        <v>36534793</v>
-      </c>
-      <c r="G59" s="47"/>
-      <c r="H59" s="48"/>
+        <v>132</v>
+      </c>
+      <c r="B59" s="38">
+        <v>6.8319999999999999</v>
+      </c>
+      <c r="C59" s="38">
+        <v>920.74599999999998</v>
+      </c>
+      <c r="D59" s="38">
+        <f>SUM(B59:C59)</f>
+        <v>927.57799999999997</v>
+      </c>
+      <c r="E59" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F59" s="39">
+        <f t="shared" si="3"/>
+        <v>26084858</v>
+      </c>
+      <c r="G59" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H59" s="45"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B60" s="40">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="C60" s="40">
-        <v>105.878</v>
-      </c>
-      <c r="D60" s="40">
-        <f t="shared" si="5"/>
-        <v>106.575</v>
-      </c>
-      <c r="E60" s="43">
-        <v>203451</v>
-      </c>
-      <c r="F60" s="42">
-        <f t="shared" si="6"/>
-        <v>36738244</v>
-      </c>
-      <c r="G60" s="47"/>
-      <c r="H60" s="48"/>
+        <v>133</v>
+      </c>
+      <c r="B60" s="38">
+        <v>6.6390000000000002</v>
+      </c>
+      <c r="C60" s="38">
+        <v>1076.6959999999999</v>
+      </c>
+      <c r="D60" s="38">
+        <f>SUM(B60:C60)</f>
+        <v>1083.3349999999998</v>
+      </c>
+      <c r="E60" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F60" s="39">
+        <f t="shared" si="3"/>
+        <v>28084858</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" s="45"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="B61" s="40">
-        <v>0.88100000000000001</v>
-      </c>
-      <c r="C61" s="40">
-        <v>131.84700000000001</v>
-      </c>
-      <c r="D61" s="40">
-        <f t="shared" si="5"/>
-        <v>132.72800000000001</v>
-      </c>
-      <c r="E61" s="43">
-        <v>272858</v>
-      </c>
-      <c r="F61" s="42">
-        <f t="shared" si="6"/>
-        <v>37011102</v>
-      </c>
-      <c r="G61" s="47"/>
-      <c r="H61" s="48"/>
+        <v>134</v>
+      </c>
+      <c r="B61" s="38">
+        <v>6.5540000000000003</v>
+      </c>
+      <c r="C61" s="38">
+        <v>588.47400000000005</v>
+      </c>
+      <c r="D61" s="38">
+        <f>SUM(B61:C61)</f>
+        <v>595.02800000000002</v>
+      </c>
+      <c r="E61" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F61" s="39">
+        <f t="shared" si="3"/>
+        <v>30084858</v>
+      </c>
+      <c r="G61" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H61" s="45"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" s="40">
-        <v>1.0840000000000001</v>
-      </c>
-      <c r="C62" s="40">
-        <v>76.88</v>
-      </c>
-      <c r="D62" s="40">
-        <f t="shared" si="5"/>
-        <v>77.963999999999999</v>
-      </c>
-      <c r="E62" s="43">
-        <v>211024</v>
-      </c>
-      <c r="F62" s="42">
-        <f t="shared" si="6"/>
-        <v>37222126</v>
-      </c>
-      <c r="G62" s="47"/>
-      <c r="H62" s="48"/>
+        <v>135</v>
+      </c>
+      <c r="B62" s="38">
+        <v>6.181</v>
+      </c>
+      <c r="C62" s="38">
+        <v>103.024</v>
+      </c>
+      <c r="D62" s="38">
+        <f>SUM(B62:C62)</f>
+        <v>109.205</v>
+      </c>
+      <c r="E62" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F62" s="39">
+        <f t="shared" si="3"/>
+        <v>32084858</v>
+      </c>
+      <c r="G62" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H62" s="45"/>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="40">
-        <v>1.2450000000000001</v>
-      </c>
-      <c r="C63" s="40">
-        <v>395.67700000000002</v>
-      </c>
-      <c r="D63" s="40">
-        <f t="shared" si="5"/>
-        <v>396.92200000000003</v>
-      </c>
-      <c r="E63" s="43">
-        <v>266053</v>
-      </c>
-      <c r="F63" s="42">
-        <f t="shared" si="6"/>
-        <v>37488179</v>
-      </c>
-      <c r="G63" s="47"/>
-      <c r="H63" s="48"/>
+        <v>136</v>
+      </c>
+      <c r="B63" s="38">
+        <v>6.26</v>
+      </c>
+      <c r="C63" s="38">
+        <v>276.38099999999997</v>
+      </c>
+      <c r="D63" s="38">
+        <f>SUM(B63:C63)</f>
+        <v>282.64099999999996</v>
+      </c>
+      <c r="E63" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F63" s="39">
+        <f t="shared" si="3"/>
+        <v>34084858</v>
+      </c>
+      <c r="G63" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H63" s="45"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="40">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="C64" s="40">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="D64" s="40">
-        <f t="shared" si="5"/>
-        <v>0.628</v>
-      </c>
-      <c r="E64" s="43">
-        <v>96</v>
-      </c>
-      <c r="F64" s="42">
-        <f t="shared" si="6"/>
-        <v>37488275</v>
-      </c>
-      <c r="G64" s="47"/>
-      <c r="H64" s="48"/>
+        <v>137</v>
+      </c>
+      <c r="B64" s="38">
+        <v>6.0919999999999996</v>
+      </c>
+      <c r="C64" s="38">
+        <v>74.933999999999997</v>
+      </c>
+      <c r="D64" s="38">
+        <f>SUM(B64:C64)</f>
+        <v>81.025999999999996</v>
+      </c>
+      <c r="E64" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F64" s="39">
+        <f t="shared" si="3"/>
+        <v>36084858</v>
+      </c>
+      <c r="G64" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H64" s="45"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="40">
-        <v>6.7809999999999997</v>
-      </c>
-      <c r="C65" s="40">
-        <v>2930.7570000000001</v>
-      </c>
-      <c r="D65" s="40">
-        <f t="shared" si="5"/>
-        <v>2937.538</v>
-      </c>
-      <c r="E65" s="42">
+        <v>138</v>
+      </c>
+      <c r="B65" s="38">
+        <v>6.2590000000000003</v>
+      </c>
+      <c r="C65" s="38">
+        <v>71.835999999999999</v>
+      </c>
+      <c r="D65" s="38">
+        <f>SUM(B65:C65)</f>
+        <v>78.094999999999999</v>
+      </c>
+      <c r="E65" s="39">
         <v>2000000</v>
       </c>
-      <c r="F65" s="42">
-        <f t="shared" si="6"/>
-        <v>39488275</v>
-      </c>
-      <c r="G65" s="47"/>
-      <c r="H65" s="48"/>
+      <c r="F65" s="39">
+        <f t="shared" si="3"/>
+        <v>38084858</v>
+      </c>
+      <c r="G65" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H65" s="45"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="40">
-        <v>6.702</v>
-      </c>
-      <c r="C66" s="40">
-        <v>2141.8389999999999</v>
-      </c>
-      <c r="D66" s="40">
-        <f t="shared" si="5"/>
-        <v>2148.5410000000002</v>
-      </c>
-      <c r="E66" s="42">
+        <v>139</v>
+      </c>
+      <c r="B66" s="38">
+        <v>6.1909999999999998</v>
+      </c>
+      <c r="C66" s="38">
+        <v>183.126</v>
+      </c>
+      <c r="D66" s="38">
+        <v>52.5</v>
+      </c>
+      <c r="E66" s="39">
         <v>2000000</v>
       </c>
-      <c r="F66" s="42">
-        <f t="shared" si="6"/>
-        <v>41488275</v>
-      </c>
-      <c r="G66" s="47"/>
-      <c r="H66" s="48"/>
+      <c r="F66" s="39">
+        <f t="shared" si="3"/>
+        <v>40084858</v>
+      </c>
+      <c r="G66" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H66" s="45"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="40">
-        <v>1.88</v>
-      </c>
-      <c r="C67" s="40">
-        <v>182.18</v>
-      </c>
-      <c r="D67" s="40">
-        <f t="shared" si="5"/>
-        <v>184.06</v>
-      </c>
-      <c r="E67" s="42">
-        <v>596583</v>
-      </c>
-      <c r="F67" s="42">
-        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="B67" s="38">
+        <v>5.7628000000000004</v>
+      </c>
+      <c r="C67" s="38">
+        <v>22.146999999999998</v>
+      </c>
+      <c r="D67" s="38">
+        <f>C67+B67</f>
+        <v>27.909799999999997</v>
+      </c>
+      <c r="E67" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F67" s="39">
+        <f t="shared" si="3"/>
         <v>42084858</v>
       </c>
-      <c r="G67" s="47"/>
-      <c r="H67" s="48"/>
+      <c r="G67" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H67" s="45"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="34"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E68" s="42"/>
-      <c r="F68" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G68" s="47"/>
-      <c r="H68" s="48"/>
+      <c r="A68" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="38">
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="C68" s="38">
+        <v>646.43799999999999</v>
+      </c>
+      <c r="D68" s="38">
+        <f t="shared" ref="D54:D76" si="4">SUM(B68:C68)</f>
+        <v>649.44299999999998</v>
+      </c>
+      <c r="E68" s="39">
+        <v>977190</v>
+      </c>
+      <c r="F68" s="39">
+        <f t="shared" si="3"/>
+        <v>43062048</v>
+      </c>
+      <c r="G68" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H68" s="45"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="34"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E69" s="42"/>
-      <c r="F69" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G69" s="47"/>
-      <c r="H69" s="48"/>
+      <c r="A69" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="38">
+        <v>0.222</v>
+      </c>
+      <c r="C69" s="38">
+        <v>8.8070000000000004</v>
+      </c>
+      <c r="D69" s="38">
+        <f t="shared" si="4"/>
+        <v>9.0289999999999999</v>
+      </c>
+      <c r="E69" s="40">
+        <v>5759</v>
+      </c>
+      <c r="F69" s="39">
+        <f t="shared" si="3"/>
+        <v>43067807</v>
+      </c>
+      <c r="G69" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H69" s="45"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="34"/>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G70" s="47"/>
-      <c r="H70" s="48"/>
+      <c r="A70" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" s="38">
+        <v>3.5760000000000001</v>
+      </c>
+      <c r="C70" s="38">
+        <v>217.29400000000001</v>
+      </c>
+      <c r="D70" s="38">
+        <f t="shared" si="4"/>
+        <v>220.87</v>
+      </c>
+      <c r="E70" s="40">
+        <v>1197721</v>
+      </c>
+      <c r="F70" s="39">
+        <f t="shared" si="3"/>
+        <v>44265528</v>
+      </c>
+      <c r="G70" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H70" s="45"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="34"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E71" s="42"/>
-      <c r="F71" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G71" s="47"/>
-      <c r="H71" s="48"/>
+      <c r="A71" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71" s="38">
+        <v>6.52</v>
+      </c>
+      <c r="C71" s="38">
+        <v>667.89800000000002</v>
+      </c>
+      <c r="D71" s="38">
+        <f t="shared" si="4"/>
+        <v>674.41800000000001</v>
+      </c>
+      <c r="E71" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F71" s="39">
+        <f t="shared" si="3"/>
+        <v>46265528</v>
+      </c>
+      <c r="G71" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H71" s="45"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="34"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E72" s="42"/>
-      <c r="F72" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G72" s="47"/>
-      <c r="H72" s="48"/>
+      <c r="A72" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B72" s="38">
+        <v>6.53</v>
+      </c>
+      <c r="C72" s="38">
+        <v>584.28300000000002</v>
+      </c>
+      <c r="D72" s="38">
+        <f t="shared" si="4"/>
+        <v>590.81299999999999</v>
+      </c>
+      <c r="E72" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F72" s="39">
+        <f t="shared" si="3"/>
+        <v>48265528</v>
+      </c>
+      <c r="G72" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H72" s="45"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="34"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E73" s="42"/>
-      <c r="F73" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G73" s="47"/>
-      <c r="H73" s="48"/>
+      <c r="A73" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="38">
+        <v>3.84</v>
+      </c>
+      <c r="C73" s="38">
+        <v>590.81399999999996</v>
+      </c>
+      <c r="D73" s="38">
+        <f t="shared" si="4"/>
+        <v>594.654</v>
+      </c>
+      <c r="E73" s="40">
+        <v>923101</v>
+      </c>
+      <c r="F73" s="39">
+        <f t="shared" si="3"/>
+        <v>49188629</v>
+      </c>
+      <c r="G73" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H73" s="45"/>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="34"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E74" s="42"/>
-      <c r="F74" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G74" s="47"/>
-      <c r="H74" s="48"/>
+      <c r="A74" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B74" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="C74" s="38">
+        <v>211.17400000000001</v>
+      </c>
+      <c r="D74" s="38">
+        <f t="shared" si="4"/>
+        <v>213.774</v>
+      </c>
+      <c r="E74" s="40">
+        <v>665114</v>
+      </c>
+      <c r="F74" s="39">
+        <f t="shared" si="3"/>
+        <v>49853743</v>
+      </c>
+      <c r="G74" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H74" s="45"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="34"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E75" s="42"/>
-      <c r="F75" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G75" s="47"/>
-      <c r="H75" s="48"/>
+      <c r="A75" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B75" s="38">
+        <v>5.9779999999999998</v>
+      </c>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38">
+        <f t="shared" si="4"/>
+        <v>5.9779999999999998</v>
+      </c>
+      <c r="E75" s="39">
+        <v>2000000</v>
+      </c>
+      <c r="F75" s="39">
+        <f t="shared" si="3"/>
+        <v>51853743</v>
+      </c>
+      <c r="G75" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="H75" s="45"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="34"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E76" s="42"/>
-      <c r="F76" s="42">
-        <f t="shared" si="6"/>
-        <v>42084858</v>
-      </c>
-      <c r="G76" s="47"/>
-      <c r="H76" s="48"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39">
+        <f t="shared" si="3"/>
+        <v>51853743</v>
+      </c>
+      <c r="G76" s="44"/>
+      <c r="H76" s="45"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="34"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38">
+        <f t="shared" ref="D77:D140" si="5">SUM(B77:C77)</f>
+        <v>0</v>
+      </c>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39">
+        <f t="shared" ref="F77:F140" si="6">F76+E77</f>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="34"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="34"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="34"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="34"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="34"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="34"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="34"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="34"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="34"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="34"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="34"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="34"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="34"/>
+      <c r="B90" s="38"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="34"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="34"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="34"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="34"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E94" s="39"/>
+      <c r="F94" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="34"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="34"/>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="39"/>
+      <c r="F96" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="34"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E97" s="39"/>
+      <c r="F97" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="34"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
+      <c r="D98" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="39"/>
+      <c r="F98" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="34"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="34"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="34"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E101" s="39"/>
+      <c r="F101" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="34"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E102" s="39"/>
+      <c r="F102" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="34"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E103" s="39"/>
+      <c r="F103" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="34"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E104" s="39"/>
+      <c r="F104" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="34"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E105" s="39"/>
+      <c r="F105" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="34"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="34"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E107" s="39"/>
+      <c r="F107" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="34"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E108" s="39"/>
+      <c r="F108" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="34"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
+      <c r="D109" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="34"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E110" s="39"/>
+      <c r="F110" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="34"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E111" s="39"/>
+      <c r="F111" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="34"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E112" s="39"/>
+      <c r="F112" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="34"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="34"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E114" s="39"/>
+      <c r="F114" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="34"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E115" s="39"/>
+      <c r="F115" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="34"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="34"/>
+      <c r="B117" s="38"/>
+      <c r="C117" s="38"/>
+      <c r="D117" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="34"/>
+      <c r="B118" s="38"/>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E118" s="39"/>
+      <c r="F118" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="34"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E119" s="39"/>
+      <c r="F119" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="34"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
+      <c r="D120" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E120" s="39"/>
+      <c r="F120" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="34"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
+      <c r="D121" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E121" s="39"/>
+      <c r="F121" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="34"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
+      <c r="D122" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E122" s="39"/>
+      <c r="F122" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="34"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E123" s="39"/>
+      <c r="F123" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="34"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E124" s="39"/>
+      <c r="F124" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="34"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E125" s="39"/>
+      <c r="F125" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="34"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E126" s="39"/>
+      <c r="F126" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="34"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E127" s="39"/>
+      <c r="F127" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="34"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="38"/>
+      <c r="D128" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E128" s="39"/>
+      <c r="F128" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="34"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="38"/>
+      <c r="D129" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E129" s="39"/>
+      <c r="F129" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="34"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="38"/>
+      <c r="D130" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E130" s="39"/>
+      <c r="F130" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="34"/>
+      <c r="B131" s="38"/>
+      <c r="C131" s="38"/>
+      <c r="D131" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E131" s="39"/>
+      <c r="F131" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="34"/>
+      <c r="B132" s="38"/>
+      <c r="C132" s="38"/>
+      <c r="D132" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E132" s="39"/>
+      <c r="F132" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="34"/>
+      <c r="B133" s="38"/>
+      <c r="C133" s="38"/>
+      <c r="D133" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E133" s="39"/>
+      <c r="F133" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="34"/>
+      <c r="B134" s="38"/>
+      <c r="C134" s="38"/>
+      <c r="D134" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E134" s="39"/>
+      <c r="F134" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="34"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="38"/>
+      <c r="D135" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E135" s="39"/>
+      <c r="F135" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="34"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="38"/>
+      <c r="D136" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E136" s="39"/>
+      <c r="F136" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="34"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
+      <c r="D137" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E137" s="39"/>
+      <c r="F137" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="34"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="38"/>
+      <c r="D138" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E138" s="39"/>
+      <c r="F138" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="34"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
+      <c r="D139" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E139" s="39"/>
+      <c r="F139" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="34"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="38"/>
+      <c r="D140" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E140" s="39"/>
+      <c r="F140" s="39">
+        <f t="shared" si="6"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="34"/>
+      <c r="B141" s="38"/>
+      <c r="C141" s="38"/>
+      <c r="D141" s="38">
+        <f t="shared" ref="D141:D147" si="7">SUM(B141:C141)</f>
+        <v>0</v>
+      </c>
+      <c r="E141" s="39"/>
+      <c r="F141" s="39">
+        <f t="shared" ref="F141:F147" si="8">F140+E141</f>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="34"/>
+      <c r="B142" s="38"/>
+      <c r="C142" s="38"/>
+      <c r="D142" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E142" s="39"/>
+      <c r="F142" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="34"/>
+      <c r="B143" s="38"/>
+      <c r="C143" s="38"/>
+      <c r="D143" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E143" s="39"/>
+      <c r="F143" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="34"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E144" s="39"/>
+      <c r="F144" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="34"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E145" s="39"/>
+      <c r="F145" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="34"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="38"/>
+      <c r="D146" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E146" s="39"/>
+      <c r="F146" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="34"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="38"/>
+      <c r="D147" s="38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E147" s="39"/>
+      <c r="F147" s="39">
+        <f t="shared" si="8"/>
+        <v>51853743</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A27:E67">
+    <sortCondition descending="1" ref="A27"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>